<commit_message>
Completed Formatting an Excel Chart
</commit_message>
<xml_diff>
--- a/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
+++ b/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/08 - Creating Basic Charts in Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A207A5DB-42F3-4A08-9029-FA640966FD9D}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83C40AE9-BAF9-47B5-ABBE-BE98747A23C7}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Monthly Budget</t>
-  </si>
   <si>
     <t>Bills</t>
   </si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>2017 Monthly Budget</t>
   </si>
 </sst>
 </file>
@@ -226,6 +226,17 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Monthly Budget'!$B$2:$H$2</c:f>
+          <c:strCache>
+            <c:ptCount val="7"/>
+            <c:pt idx="0">
+              <c:v>2017 Monthly Budget</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -278,7 +289,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -736,7 +747,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -794,7 +805,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -822,7 +833,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -836,7 +847,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4865,8 +4876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4878,7 +4889,7 @@
   <sheetData>
     <row r="2" spans="2:8" ht="37" x14ac:dyDescent="1.05">
       <c r="B2" s="7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4889,7 +4900,7 @@
     </row>
     <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
         <v>42736</v>
@@ -4904,15 +4915,15 @@
         <v>42826</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>1200</v>
@@ -4937,7 +4948,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2">
         <v>100</v>
@@ -4962,7 +4973,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
         <v>150</v>
@@ -4987,7 +4998,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>50</v>
@@ -5012,7 +5023,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2">
         <v>200</v>
@@ -5037,7 +5048,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>100</v>
@@ -5062,7 +5073,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <f>SUM(C5:C10)</f>
@@ -5091,7 +5102,7 @@
     </row>
     <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <f>MIN(C5:C10)</f>
@@ -5108,7 +5119,7 @@
     </row>
     <row r="14" spans="2:8" ht="16" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <f>MAX(C5:C10)</f>
@@ -5125,7 +5136,7 @@
     </row>
     <row r="15" spans="2:8" ht="16" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <f>AVERAGE(C5:C10)</f>
@@ -5142,7 +5153,7 @@
     </row>
     <row r="16" spans="2:8" ht="16" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <f>COUNT(C5:C10)</f>

</xml_diff>

<commit_message>
Completed Moving a Chart to another Worksheet
</commit_message>
<xml_diff>
--- a/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
+++ b/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/08 - Creating Basic Charts in Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83C40AE9-BAF9-47B5-ABBE-BE98747A23C7}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{582B8399-9D96-4F72-99E0-BEAB7AC011F3}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart Monthly Budget" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -341,7 +342,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000000-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -413,7 +414,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000001-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -485,7 +486,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000002-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -557,7 +558,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000003-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -629,7 +630,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000004-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -701,7 +702,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-0D66-4909-A9A9-CE01136E90FC}"/>
+              <c16:uniqueId val="{00000005-3F59-43F1-94BE-5082D2972BD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -899,11 +900,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1448,6 +1444,17 @@
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{58676EAF-BDB3-4949-BA5B-512D8B0C6B19}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="60" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4518,29 +4525,26 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>234042</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>183242</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>540656</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>187778</xdr:rowOff>
-    </xdr:to>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7430325" cy="5393377"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05E4D94F-D78D-C08F-BE00-DF6741E20E82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3D0C515-E16C-812C-FB5E-F352F911F716}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4548,12 +4552,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4876,8 +4880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Completed Viewing your Document in Print Preview
</commit_message>
<xml_diff>
--- a/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
+++ b/08 - Creating Basic Charts in Excel/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/08 - Creating Basic Charts in Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{582B8399-9D96-4F72-99E0-BEAB7AC011F3}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BABA2F2A-F6A9-44B9-9684-9A9C0BF51CE2}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,6 +213,369 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Monthly Budget'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Monthly Budget'!$B$5:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Phone</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Credit Cards</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Candy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Monthly Budget'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ ">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B65C-4FB7-BD81-895570032D02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -943,7 +1306,566 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4525,6 +5447,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>216806</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>70755</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>524327</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>75291</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478D8A87-818B-4157-409B-6C639ABD81D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4880,8 +5838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>